<commit_message>
Refactor and enhance MVVM architecture
- Updated `UpdateTextBlockEvents.cs` to handle nullable strings.
- Refactored dependency injection to use `IWindowFactory<T>`.
- Introduced `ViewModelBase` and `RelayCommands` for MVVM.
- Added `EditLoadFilesModel` and `SettingViewModel` for better UI logic.
- Replaced event handlers with command bindings in XAML files.
- Improved resource management in `FindMissingProducts.cs`.
- Moved `LangCodeAttribute` and enums to `Core` namespace.
- Added `EnumHelper` for enum utilities and descriptions.
- Updated `AppSettings` to support robust language handling.
- Simplified and cleaned up project files and namespaces.
</commit_message>
<xml_diff>
--- a/ExcelShSy.Infrastcarture.Tests/Files/priceTemplate.xlsx
+++ b/ExcelShSy.Infrastcarture.Tests/Files/priceTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Freid\source\repos\FreidFry\ExcelShopSync\ExcelShSy.Infrastcarture.Tests\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D894D9F-6057-4284-98E7-35F4DB52D95A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895B1C1A-0231-468E-BCFB-BB41E3CC9131}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8430" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Settings" sheetId="22" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$6</definedName>
     <definedName name="Наличие_Товаров">Наличие[Наличие_Товаров]</definedName>
     <definedName name="Столбец_Артикула" comment="ОБЯЗАТЕЛЬНО БЕЗ ПОВТОРЕНИЙ. НЕЛЬЗЯ 2 ОДИНАКОВЫХ ВАРИАНТА">Settings!$A$10:$A$11</definedName>
     <definedName name="Столбец_Наличия" comment="ОБЯЗАТЕЛЬНО БЕЗ ПОВТОРЕНИЙ. НЕЛЬЗЯ 2 ОДИНАКОВЫХ ВАРИАНТА">Settings!$A$14:$A$15</definedName>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>Артикул</t>
   </si>
@@ -103,13 +103,19 @@
   </si>
   <si>
     <t>TEST PRODUCT IN THREE LAYER AND SPACES</t>
+  </si>
+  <si>
+    <t>Formula10_000mult0.3</t>
+  </si>
+  <si>
+    <t>Formula_10_000multi3.33333</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -150,6 +156,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -280,7 +294,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -312,6 +326,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,8 +426,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A7D702B-B514-44D6-BCDA-3B8002F7FE47}" name="Дашок" displayName="Дашок" ref="A1:F5" headerRowDxfId="3">
-  <autoFilter ref="A1:F5" xr:uid="{5223FFCF-4A5B-424C-9234-F8859BD87B20}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A7D702B-B514-44D6-BCDA-3B8002F7FE47}" name="Дашок" displayName="Дашок" ref="A1:F6" headerRowDxfId="3">
+  <autoFilter ref="A1:F6" xr:uid="{5223FFCF-4A5B-424C-9234-F8859BD87B20}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -654,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -851,6 +870,38 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1">
+      <c r="A6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1">
+        <f>10000*G7</f>
+        <v>33333.300000000003</v>
+      </c>
+      <c r="C6" s="13" t="str">
+        <f>$I$3</f>
+        <v>Под заказ</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="18">
+        <f>10000*G6</f>
+        <v>3000</v>
+      </c>
+      <c r="F6" s="13" t="str">
+        <f>$I$2</f>
+        <v>Нет в наличии</v>
+      </c>
+      <c r="G6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1">
+      <c r="G7">
+        <v>3.3333300000000001</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:C5">
     <sortCondition ref="B2:B5"/>
@@ -873,7 +924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D023C29-C9E5-44FE-A734-A016AEFDF45A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>